<commit_message>
updating analytics layer with agg/granular for gold
</commit_message>
<xml_diff>
--- a/bronze/excel/stg_aircraft.xlsx
+++ b/bronze/excel/stg_aircraft.xlsx
@@ -487,17 +487,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AC7432</t>
+          <t>AC6692</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Boeing 737-800</t>
+          <t>Airbus A321XLR</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Boeing</t>
+          <t>Airbus</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -506,10 +506,10 @@
         </is>
       </c>
       <c r="E2" t="n">
-        <v>2007</v>
+        <v>2015</v>
       </c>
       <c r="F2" t="n">
-        <v>160</v>
+        <v>183</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -517,16 +517,16 @@
         </is>
       </c>
       <c r="H2" t="n">
-        <v>850</v>
+        <v>890</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>AC9250</t>
+          <t>AC9548</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -545,10 +545,10 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>2016</v>
+        <v>2020</v>
       </c>
       <c r="F3" t="n">
-        <v>199</v>
+        <v>182</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -559,35 +559,35 @@
         <v>1000</v>
       </c>
       <c r="I3" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AC4709</t>
+          <t>AC5545</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Airbus A350-900</t>
+          <t>Boeing 757-200</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Airbus</t>
+          <t>Boeing</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>wide-body</t>
+          <t>narrow-body</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>2014</v>
+        <v>2007</v>
       </c>
       <c r="F4" t="n">
-        <v>287</v>
+        <v>194</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -595,21 +595,21 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>1350</v>
+        <v>1000</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>AC7421</t>
+          <t>AC5517</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Airbus A321XLR</t>
+          <t>Airbus A350-900</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -619,14 +619,14 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>narrow-body</t>
+          <t>wide-body</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="F5" t="n">
-        <v>192</v>
+        <v>294</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -634,21 +634,21 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>890</v>
+        <v>1350</v>
       </c>
       <c r="I5" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>AC7979</t>
+          <t>AC3879</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>CRJ700</t>
+          <t>Embraer E175</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -662,10 +662,10 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>2007</v>
+        <v>2013</v>
       </c>
       <c r="F6" t="n">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -673,16 +673,16 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>500</v>
+        <v>550</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>AC5682</t>
+          <t>AC4392</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -701,10 +701,10 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>2009</v>
+        <v>2015</v>
       </c>
       <c r="F7" t="n">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -715,35 +715,35 @@
         <v>790</v>
       </c>
       <c r="I7" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>AC4686</t>
+          <t>AC6192</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Airbus A350-900</t>
+          <t>Embraer E175</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Airbus</t>
+          <t>Boeing</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>wide-body</t>
+          <t>regional jet</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>2008</v>
+        <v>2018</v>
       </c>
       <c r="F8" t="n">
-        <v>307</v>
+        <v>81</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -751,26 +751,26 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>1350</v>
+        <v>550</v>
       </c>
       <c r="I8" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>AC8469</t>
+          <t>AC2035</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Boeing 777-300ER</t>
+          <t>Airbus A350-900</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Boeing</t>
+          <t>Airbus</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -779,10 +779,10 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="F9" t="n">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -790,21 +790,21 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>1600</v>
+        <v>1350</v>
       </c>
       <c r="I9" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>AC2907</t>
+          <t>AC7731</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Airbus A350-900</t>
+          <t>Airbus A350-1000</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -818,10 +818,10 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>2021</v>
+        <v>2008</v>
       </c>
       <c r="F10" t="n">
-        <v>323</v>
+        <v>397</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -829,21 +829,21 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>1350</v>
+        <v>1450</v>
       </c>
       <c r="I10" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>AC4674</t>
+          <t>AC2692</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Airbus A350-900</t>
+          <t>Airbus A320neo</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -853,14 +853,14 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>wide-body</t>
+          <t>narrow-body</t>
         </is>
       </c>
       <c r="E11" t="n">
         <v>2017</v>
       </c>
       <c r="F11" t="n">
-        <v>324</v>
+        <v>152</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -868,38 +868,38 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>1350</v>
+        <v>790</v>
       </c>
       <c r="I11" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>AC4266</t>
+          <t>AC7504</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Airbus A350-1000</t>
+          <t>Embraer E175</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Airbus</t>
+          <t>Boeing</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>wide-body</t>
+          <t>regional jet</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="F12" t="n">
-        <v>381</v>
+        <v>78</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -907,26 +907,26 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>1450</v>
+        <v>550</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>AC9894</t>
+          <t>AC9038</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Airbus A321XLR</t>
+          <t>Boeing 757-200</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Airbus</t>
+          <t>Boeing</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -935,10 +935,10 @@
         </is>
       </c>
       <c r="E13" t="n">
-        <v>2018</v>
+        <v>2022</v>
       </c>
       <c r="F13" t="n">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -946,38 +946,38 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>890</v>
+        <v>1000</v>
       </c>
       <c r="I13" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>AC2808</t>
+          <t>AC5387</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Airbus A320neo</t>
+          <t>CRJ700</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Airbus</t>
+          <t>Boeing</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>narrow-body</t>
+          <t>regional jet</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>2014</v>
+        <v>2018</v>
       </c>
       <c r="F14" t="n">
-        <v>171</v>
+        <v>71</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -985,26 +985,26 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>790</v>
+        <v>500</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>AC7608</t>
+          <t>AC1586</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Airbus A321XLR</t>
+          <t>Boeing 737-800</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Airbus</t>
+          <t>Boeing</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -1013,10 +1013,10 @@
         </is>
       </c>
       <c r="E15" t="n">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="F15" t="n">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1024,21 +1024,21 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>890</v>
+        <v>850</v>
       </c>
       <c r="I15" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>AC7459</t>
+          <t>AC9717</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Airbus A320neo</t>
+          <t>Airbus A350-1000</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1048,14 +1048,14 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>narrow-body</t>
+          <t>wide-body</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>2005</v>
+        <v>2006</v>
       </c>
       <c r="F16" t="n">
-        <v>180</v>
+        <v>387</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -1063,10 +1063,10 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>790</v>
+        <v>1450</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>45840</v>
+        <v>45863</v>
       </c>
     </row>
   </sheetData>

</xml_diff>